<commit_message>
atualizei a variavel camarades10, de acordo com a regra: se relatou FSTprotocol e method_measurement "yes", se relatou apenas um "unclear e se não relatou ambos "no".
</commit_message>
<xml_diff>
--- a/data/conferencia.xlsx
+++ b/data/conferencia.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4" documentId="11_BA6C1DC68F79A8D366075C52F37BD272BAC13030" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2838111E-ABB7-4B2B-BF11-6900B4F34BA2}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1141,7 +1141,7 @@
   <dimension ref="A1:C205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>